<commit_message>
[MOSIP-21520] update mosip-data for hindi,kannada, and tamil language
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/blacklisted_words.xlsx
+++ b/mosip_master/xlsx/blacklisted_words.xlsx
@@ -94,7 +94,7 @@
     <t xml:space="preserve">ಡ್ಯಾಮ್</t>
   </si>
   <si>
-    <t xml:space="preserve"> ನಿಗ್ಗಾ</t>
+    <t xml:space="preserve">ನಿಗ್ಗಾ</t>
   </si>
   <si>
     <t xml:space="preserve">ಡ್ಯಾಮಿಟ್</t>
@@ -115,7 +115,7 @@
     <t xml:space="preserve">निग्गा</t>
   </si>
   <si>
-    <t xml:space="preserve"> दमित</t>
+    <t xml:space="preserve">दमित</t>
   </si>
   <si>
     <t xml:space="preserve">tam</t>
@@ -266,7 +266,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Configure test data modification
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/blacklisted_words.xlsx
+++ b/mosip_master/xlsx/blacklisted_words.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balaji.Alluru\Desktop\Mosip\GitHub\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MicroTech\IdeaProjects\mosip-data-mec\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AFACA3-D4A5-4158-A4ED-32C32422EE5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>lang_code</t>
   </si>
@@ -51,12 +52,6 @@
   </si>
   <si>
     <t>damn</t>
-  </si>
-  <si>
-    <t>nigga</t>
-  </si>
-  <si>
-    <t>dammit</t>
   </si>
   <si>
     <t>fra</t>
@@ -89,7 +84,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -432,21 +427,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="1"/>
+    <col min="3" max="3" width="30.44140625" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -460,7 +455,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -474,7 +469,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -488,112 +483,84 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="B6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="B7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D11"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D12"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>